<commit_message>
feat: parametro de componente_financiacion para controlar variables de curvas y productos
</commit_message>
<xml_diff>
--- a/prototipo_pcr/inputs/insumos.xlsx
+++ b/prototipo_pcr/inputs/insumos.xlsx
@@ -8,40 +8,41 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\proyectos_sura\Decenal\Prototipo\prototipo-pcr\prototipo_pcr\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553378E1-7C27-4AC0-B444-096812339665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2243AF27-2D62-4BE1-9706-CB09D188EEFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="959" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="param_contabilidad" sheetId="6" r:id="rId1"/>
     <sheet name="excepciones_50_50" sheetId="4" r:id="rId2"/>
-    <sheet name="gastos" sheetId="1" r:id="rId3"/>
-    <sheet name="tasa_cambio" sheetId="3" r:id="rId4"/>
-    <sheet name="porc_descuento" sheetId="5" r:id="rId5"/>
-    <sheet name="produccion_directo" sheetId="9" r:id="rId6"/>
-    <sheet name="componente_inversion_directo" sheetId="28" r:id="rId7"/>
-    <sheet name="produccion_rea" sheetId="2" r:id="rId8"/>
-    <sheet name="comision_rea" sheetId="18" r:id="rId9"/>
-    <sheet name="costo_rea_noprop" sheetId="8" r:id="rId10"/>
-    <sheet name="seguimiento_rea_noprop" sheetId="19" r:id="rId11"/>
-    <sheet name="onerosidad" sheetId="26" r:id="rId12"/>
-    <sheet name="recup_onerosidad" sheetId="27" r:id="rId13"/>
-    <sheet name="map_bt" sheetId="20" r:id="rId14"/>
-    <sheet name="tipo_seguro" sheetId="21" r:id="rId15"/>
-    <sheet name="cuenta_cobrar_directo" sheetId="23" r:id="rId16"/>
-    <sheet name="cuenta_corriente_rea" sheetId="25" r:id="rId17"/>
+    <sheet name="componente_financiacion" sheetId="29" r:id="rId3"/>
+    <sheet name="gastos" sheetId="1" r:id="rId4"/>
+    <sheet name="tasa_cambio" sheetId="3" r:id="rId5"/>
+    <sheet name="porc_descuento" sheetId="5" r:id="rId6"/>
+    <sheet name="produccion_directo" sheetId="9" r:id="rId7"/>
+    <sheet name="componente_inversion_directo" sheetId="28" r:id="rId8"/>
+    <sheet name="produccion_rea" sheetId="2" r:id="rId9"/>
+    <sheet name="comision_rea" sheetId="18" r:id="rId10"/>
+    <sheet name="costo_rea_noprop" sheetId="8" r:id="rId11"/>
+    <sheet name="seguimiento_rea_noprop" sheetId="19" r:id="rId12"/>
+    <sheet name="onerosidad" sheetId="26" r:id="rId13"/>
+    <sheet name="recup_onerosidad" sheetId="27" r:id="rId14"/>
+    <sheet name="map_bt" sheetId="20" r:id="rId15"/>
+    <sheet name="tipo_seguro" sheetId="21" r:id="rId16"/>
+    <sheet name="cuenta_cobrar_directo" sheetId="23" r:id="rId17"/>
+    <sheet name="cuenta_corriente_rea" sheetId="25" r:id="rId18"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">comision_rea!$A$1:$V$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">componente_inversion_directo!$A$1:$W$37</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">gastos!$B$1:$K$221</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">map_bt!$A$1:$I$261</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">comision_rea!$A$1:$V$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">componente_inversion_directo!$A$1:$W$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">gastos!$B$1:$K$221</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">map_bt!$A$1:$I$261</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">param_contabilidad!$A$1:$J$86</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">porc_descuento!$A$1:$N$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">produccion_directo!$A$1:$V$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">produccion_rea!$A$1:$AB$10</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">tasa_cambio!$A$1:$D$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">tipo_seguro!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">porc_descuento!$A$1:$N$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">produccion_directo!$A$1:$V$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">produccion_rea!$A$1:$AB$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">tasa_cambio!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">tipo_seguro!$A$1:$C$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -1037,7 +1038,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8937" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8963" uniqueCount="457">
   <si>
     <t>tipo_insumo</t>
   </si>
@@ -2391,6 +2392,24 @@
   <si>
     <t>VIVIENDA_SEGURA</t>
   </si>
+  <si>
+    <t>moneda_curva</t>
+  </si>
+  <si>
+    <t>UVR</t>
+  </si>
+  <si>
+    <t>aplica_comp_financ</t>
+  </si>
+  <si>
+    <t>meses_max_vigencia</t>
+  </si>
+  <si>
+    <t>pais_curva</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
 </sst>
 </file>
 
@@ -2402,7 +2421,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -2692,7 +2711,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Millares" xfId="5" builtinId="3"/>
@@ -3038,7 +3057,7 @@
   </sheetPr>
   <dimension ref="A1:K89"/>
   <sheetViews>
-    <sheetView topLeftCell="B6" zoomScale="101" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="101" workbookViewId="0">
       <selection activeCell="G23" sqref="G23:G25"/>
     </sheetView>
   </sheetViews>
@@ -5911,6 +5930,709 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED59B340-08CC-1E4C-83CE-42156F1868E1}">
+  <sheetPr codeName="Hoja8"/>
+  <dimension ref="A1:X9"/>
+  <sheetViews>
+    <sheetView zoomScale="109" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:K1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="25.21875" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.44140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.44140625" customWidth="1"/>
+    <col min="19" max="19" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="26.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" s="5" customFormat="1">
+      <c r="A1" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="F1" s="49" t="s">
+        <v>163</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="J1" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" s="49" t="s">
+        <v>74</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2">
+        <v>1111</v>
+      </c>
+      <c r="D2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2">
+        <v>2374188</v>
+      </c>
+      <c r="F2" t="s">
+        <v>169</v>
+      </c>
+      <c r="G2">
+        <v>0.4</v>
+      </c>
+      <c r="H2">
+        <v>6720148806</v>
+      </c>
+      <c r="I2" s="14">
+        <v>45108</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="L2">
+        <v>124324091</v>
+      </c>
+      <c r="M2" t="s">
+        <v>124</v>
+      </c>
+      <c r="N2">
+        <v>124324511</v>
+      </c>
+      <c r="O2" t="s">
+        <v>96</v>
+      </c>
+      <c r="P2" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>114</v>
+      </c>
+      <c r="R2" s="4">
+        <v>45292</v>
+      </c>
+      <c r="S2" s="4">
+        <v>45306</v>
+      </c>
+      <c r="T2" s="4">
+        <v>45672</v>
+      </c>
+      <c r="U2" s="4">
+        <v>45306</v>
+      </c>
+      <c r="V2" s="4">
+        <v>45672</v>
+      </c>
+      <c r="W2">
+        <v>120</v>
+      </c>
+      <c r="X2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
+      <c r="A3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3">
+        <v>1111</v>
+      </c>
+      <c r="D3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3">
+        <v>6987458</v>
+      </c>
+      <c r="F3" t="s">
+        <v>169</v>
+      </c>
+      <c r="G3">
+        <v>0.3</v>
+      </c>
+      <c r="H3">
+        <v>3517986098</v>
+      </c>
+      <c r="I3" s="14">
+        <v>45108</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="L3">
+        <v>124324091</v>
+      </c>
+      <c r="M3" t="s">
+        <v>124</v>
+      </c>
+      <c r="N3">
+        <v>124324511</v>
+      </c>
+      <c r="O3" t="s">
+        <v>96</v>
+      </c>
+      <c r="P3" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>114</v>
+      </c>
+      <c r="R3" s="4">
+        <v>45292</v>
+      </c>
+      <c r="S3" s="4">
+        <v>45306</v>
+      </c>
+      <c r="T3" s="4">
+        <v>45672</v>
+      </c>
+      <c r="U3" s="4">
+        <v>45306</v>
+      </c>
+      <c r="V3" s="4">
+        <v>45672</v>
+      </c>
+      <c r="W3">
+        <v>120</v>
+      </c>
+      <c r="X3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
+      <c r="A4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4">
+        <v>1111</v>
+      </c>
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4">
+        <v>3693358</v>
+      </c>
+      <c r="F4" t="s">
+        <v>170</v>
+      </c>
+      <c r="G4">
+        <v>0.3</v>
+      </c>
+      <c r="H4">
+        <v>1944219246</v>
+      </c>
+      <c r="I4" s="14">
+        <v>45108</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="L4">
+        <v>124324091</v>
+      </c>
+      <c r="M4" t="s">
+        <v>124</v>
+      </c>
+      <c r="N4">
+        <v>124324511</v>
+      </c>
+      <c r="O4" t="s">
+        <v>96</v>
+      </c>
+      <c r="P4" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>114</v>
+      </c>
+      <c r="R4" s="4">
+        <v>45292</v>
+      </c>
+      <c r="S4" s="4">
+        <v>45306</v>
+      </c>
+      <c r="T4" s="4">
+        <v>45672</v>
+      </c>
+      <c r="U4" s="4">
+        <v>45306</v>
+      </c>
+      <c r="V4" s="4">
+        <v>45672</v>
+      </c>
+      <c r="W4">
+        <v>120</v>
+      </c>
+      <c r="X4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
+      <c r="A5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5">
+        <v>1111</v>
+      </c>
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5">
+        <v>2374188</v>
+      </c>
+      <c r="F5" t="s">
+        <v>169</v>
+      </c>
+      <c r="G5">
+        <v>0.4</v>
+      </c>
+      <c r="H5">
+        <v>5249897308</v>
+      </c>
+      <c r="I5" s="14">
+        <v>45108</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="L5">
+        <v>124324092</v>
+      </c>
+      <c r="M5" t="s">
+        <v>124</v>
+      </c>
+      <c r="N5">
+        <v>124324512</v>
+      </c>
+      <c r="O5" t="s">
+        <v>96</v>
+      </c>
+      <c r="P5" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>115</v>
+      </c>
+      <c r="R5" s="4">
+        <v>45245</v>
+      </c>
+      <c r="S5" s="4">
+        <v>45306</v>
+      </c>
+      <c r="T5" s="4">
+        <v>45672</v>
+      </c>
+      <c r="U5" s="4">
+        <v>45306</v>
+      </c>
+      <c r="V5" s="4">
+        <v>45672</v>
+      </c>
+      <c r="W5">
+        <v>120</v>
+      </c>
+      <c r="X5">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
+      <c r="A6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6">
+        <v>1111</v>
+      </c>
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6">
+        <v>6987458</v>
+      </c>
+      <c r="F6" t="s">
+        <v>169</v>
+      </c>
+      <c r="G6">
+        <v>0.3</v>
+      </c>
+      <c r="H6">
+        <v>4579088313</v>
+      </c>
+      <c r="I6" s="14">
+        <v>45108</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="L6">
+        <v>124324092</v>
+      </c>
+      <c r="M6" t="s">
+        <v>124</v>
+      </c>
+      <c r="N6">
+        <v>124324512</v>
+      </c>
+      <c r="O6" t="s">
+        <v>96</v>
+      </c>
+      <c r="P6" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>115</v>
+      </c>
+      <c r="R6" s="4">
+        <v>45245</v>
+      </c>
+      <c r="S6" s="4">
+        <v>45306</v>
+      </c>
+      <c r="T6" s="4">
+        <v>45672</v>
+      </c>
+      <c r="U6" s="4">
+        <v>45306</v>
+      </c>
+      <c r="V6" s="4">
+        <v>45672</v>
+      </c>
+      <c r="W6">
+        <v>120</v>
+      </c>
+      <c r="X6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24">
+      <c r="A7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7">
+        <v>1111</v>
+      </c>
+      <c r="D7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7">
+        <v>3693358</v>
+      </c>
+      <c r="F7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G7">
+        <v>0.3</v>
+      </c>
+      <c r="H7">
+        <v>7859725531</v>
+      </c>
+      <c r="I7" s="14">
+        <v>45108</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="L7">
+        <v>124324092</v>
+      </c>
+      <c r="M7" t="s">
+        <v>124</v>
+      </c>
+      <c r="N7">
+        <v>124324512</v>
+      </c>
+      <c r="O7" t="s">
+        <v>96</v>
+      </c>
+      <c r="P7" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>115</v>
+      </c>
+      <c r="R7" s="4">
+        <v>45245</v>
+      </c>
+      <c r="S7" s="4">
+        <v>45306</v>
+      </c>
+      <c r="T7" s="4">
+        <v>45672</v>
+      </c>
+      <c r="U7" s="4">
+        <v>45306</v>
+      </c>
+      <c r="V7" s="4">
+        <v>45672</v>
+      </c>
+      <c r="W7">
+        <v>120</v>
+      </c>
+      <c r="X7">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24">
+      <c r="A8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8">
+        <v>1245</v>
+      </c>
+      <c r="D8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8">
+        <v>3693358</v>
+      </c>
+      <c r="F8" t="s">
+        <v>170</v>
+      </c>
+      <c r="G8">
+        <v>0.5</v>
+      </c>
+      <c r="H8">
+        <v>5260869017</v>
+      </c>
+      <c r="I8" s="14">
+        <v>45292</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="L8">
+        <v>345675387</v>
+      </c>
+      <c r="M8" t="s">
+        <v>127</v>
+      </c>
+      <c r="N8">
+        <v>345675807</v>
+      </c>
+      <c r="O8" t="s">
+        <v>91</v>
+      </c>
+      <c r="P8" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>115</v>
+      </c>
+      <c r="R8" s="4">
+        <v>45342</v>
+      </c>
+      <c r="S8" s="4">
+        <v>45306</v>
+      </c>
+      <c r="T8" s="4">
+        <v>45337</v>
+      </c>
+      <c r="U8" s="4">
+        <v>45306</v>
+      </c>
+      <c r="V8" s="4">
+        <v>45337</v>
+      </c>
+      <c r="W8">
+        <v>6</v>
+      </c>
+      <c r="X8">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24">
+      <c r="A9" t="s">
+        <v>147</v>
+      </c>
+      <c r="B9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9">
+        <v>1245</v>
+      </c>
+      <c r="D9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9">
+        <v>2374188</v>
+      </c>
+      <c r="F9" t="s">
+        <v>169</v>
+      </c>
+      <c r="G9">
+        <v>0.5</v>
+      </c>
+      <c r="H9">
+        <v>1292794322</v>
+      </c>
+      <c r="I9" s="14">
+        <v>45292</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="L9">
+        <v>345675387</v>
+      </c>
+      <c r="M9" t="s">
+        <v>127</v>
+      </c>
+      <c r="N9">
+        <v>345675807</v>
+      </c>
+      <c r="O9" t="s">
+        <v>91</v>
+      </c>
+      <c r="P9" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>115</v>
+      </c>
+      <c r="R9" s="4">
+        <v>45342</v>
+      </c>
+      <c r="S9" s="4">
+        <v>45306</v>
+      </c>
+      <c r="T9" s="4">
+        <v>45337</v>
+      </c>
+      <c r="U9" s="4">
+        <v>45306</v>
+      </c>
+      <c r="V9" s="4">
+        <v>45337</v>
+      </c>
+      <c r="W9">
+        <v>6</v>
+      </c>
+      <c r="X9">
+        <v>0.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B056C4-8D76-6947-BFDD-DD6636C4305C}">
   <sheetPr codeName="Hoja9"/>
   <dimension ref="A1:U6"/>
@@ -6336,7 +7058,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1087A3BC-C506-2548-A2C0-B6F2D6615AC0}">
   <sheetPr codeName="Hoja10"/>
   <dimension ref="A1:L35"/>
@@ -7372,7 +8094,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20B783E5-A0C2-5D46-A94A-481A8E8B68D6}">
   <sheetPr codeName="Hoja11"/>
   <dimension ref="A1:Y5"/>
@@ -7814,7 +8536,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{749D5A92-E07C-E345-9059-987184A894F0}">
   <sheetPr codeName="Hoja12"/>
   <dimension ref="A1:P4"/>
@@ -8052,7 +8774,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A12977D-9D3C-784D-BA64-82A8AADC1B2E}">
   <sheetPr codeName="Hoja13">
     <tabColor theme="4"/>
@@ -14871,7 +15593,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FB4049-F651-384C-8DCF-CEAFB17703EB}">
   <sheetPr codeName="Hoja14">
     <tabColor theme="4"/>
@@ -15570,7 +16292,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F7F059E-3482-9948-A0EE-3B780BE80211}">
   <sheetPr codeName="Hoja15">
     <tabColor rgb="FFC00000"/>
@@ -15841,7 +16563,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C59D3D0B-BDA7-C849-9A02-F348974FBECC}">
   <sheetPr codeName="Hoja16">
     <tabColor rgb="FFC00000"/>
@@ -16033,7 +16755,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScale="135" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F3"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -16174,15 +16896,141 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BBAE1AE-0ED6-4B2E-B092-2639765DD066}">
+  <sheetPr>
+    <tabColor theme="9"/>
+  </sheetPr>
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.77734375" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="5" customFormat="1">
+      <c r="A1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>451</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="10" customFormat="1">
+      <c r="A2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>342</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="10">
+        <v>1</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>456</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>452</v>
+      </c>
+      <c r="J2" s="10">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="10" customFormat="1">
+      <c r="A3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>342</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" s="10">
+        <v>1</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>456</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>452</v>
+      </c>
+      <c r="J3" s="10">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja3">
     <tabColor theme="4"/>
   </sheetPr>
   <dimension ref="A1:M245"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.21875" defaultRowHeight="14.4"/>
@@ -26255,7 +27103,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{787BB09D-1F62-C94C-AC6C-8ED6FF77D608}">
   <sheetPr codeName="Hoja4"/>
   <dimension ref="A1:E1462"/>
@@ -47799,7 +48647,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF3E8B5B-0165-4DAB-BED5-73CFCF40B2AB}">
   <sheetPr codeName="Hoja5"/>
   <dimension ref="A1:N37"/>
@@ -48660,7 +49508,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3AB633E-9AEE-C044-8F09-ED4F88978E4B}">
   <sheetPr codeName="Hoja6"/>
   <dimension ref="A1:V25"/>
@@ -50379,7 +51227,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91DF4D8-2AEA-4913-93D7-B86EA85C5B3E}">
   <dimension ref="A1:W41"/>
   <sheetViews>
@@ -53018,7 +53866,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F93C6E-21BF-4220-AF0D-6D307F3158B8}">
   <sheetPr codeName="Hoja7"/>
   <dimension ref="A1:AD11"/>
@@ -54107,721 +54955,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED59B340-08CC-1E4C-83CE-42156F1868E1}">
-  <sheetPr codeName="Hoja8"/>
-  <dimension ref="A1:X9"/>
-  <sheetViews>
-    <sheetView zoomScale="109" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:K1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="25.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="25.21875" customWidth="1"/>
-    <col min="8" max="8" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.44140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.44140625" customWidth="1"/>
-    <col min="19" max="19" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="26.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:24" s="5" customFormat="1">
-      <c r="A1" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="B1" s="49" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="D1" s="49" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="F1" s="49" t="s">
-        <v>163</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="J1" s="49" t="s">
-        <v>73</v>
-      </c>
-      <c r="K1" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="W1" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24">
-      <c r="A2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2">
-        <v>1111</v>
-      </c>
-      <c r="D2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2">
-        <v>2374188</v>
-      </c>
-      <c r="F2" t="s">
-        <v>169</v>
-      </c>
-      <c r="G2">
-        <v>0.4</v>
-      </c>
-      <c r="H2">
-        <v>6720148806</v>
-      </c>
-      <c r="I2" s="14">
-        <v>45108</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="L2">
-        <v>124324091</v>
-      </c>
-      <c r="M2" t="s">
-        <v>124</v>
-      </c>
-      <c r="N2">
-        <v>124324511</v>
-      </c>
-      <c r="O2" t="s">
-        <v>96</v>
-      </c>
-      <c r="P2" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>114</v>
-      </c>
-      <c r="R2" s="4">
-        <v>45292</v>
-      </c>
-      <c r="S2" s="4">
-        <v>45306</v>
-      </c>
-      <c r="T2" s="4">
-        <v>45672</v>
-      </c>
-      <c r="U2" s="4">
-        <v>45306</v>
-      </c>
-      <c r="V2" s="4">
-        <v>45672</v>
-      </c>
-      <c r="W2">
-        <v>120</v>
-      </c>
-      <c r="X2">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24">
-      <c r="A3" t="s">
-        <v>152</v>
-      </c>
-      <c r="B3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3">
-        <v>1111</v>
-      </c>
-      <c r="D3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3">
-        <v>6987458</v>
-      </c>
-      <c r="F3" t="s">
-        <v>169</v>
-      </c>
-      <c r="G3">
-        <v>0.3</v>
-      </c>
-      <c r="H3">
-        <v>3517986098</v>
-      </c>
-      <c r="I3" s="14">
-        <v>45108</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="L3">
-        <v>124324091</v>
-      </c>
-      <c r="M3" t="s">
-        <v>124</v>
-      </c>
-      <c r="N3">
-        <v>124324511</v>
-      </c>
-      <c r="O3" t="s">
-        <v>96</v>
-      </c>
-      <c r="P3" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>114</v>
-      </c>
-      <c r="R3" s="4">
-        <v>45292</v>
-      </c>
-      <c r="S3" s="4">
-        <v>45306</v>
-      </c>
-      <c r="T3" s="4">
-        <v>45672</v>
-      </c>
-      <c r="U3" s="4">
-        <v>45306</v>
-      </c>
-      <c r="V3" s="4">
-        <v>45672</v>
-      </c>
-      <c r="W3">
-        <v>120</v>
-      </c>
-      <c r="X3">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24">
-      <c r="A4" t="s">
-        <v>152</v>
-      </c>
-      <c r="B4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4">
-        <v>1111</v>
-      </c>
-      <c r="D4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4">
-        <v>3693358</v>
-      </c>
-      <c r="F4" t="s">
-        <v>170</v>
-      </c>
-      <c r="G4">
-        <v>0.3</v>
-      </c>
-      <c r="H4">
-        <v>1944219246</v>
-      </c>
-      <c r="I4" s="14">
-        <v>45108</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="L4">
-        <v>124324091</v>
-      </c>
-      <c r="M4" t="s">
-        <v>124</v>
-      </c>
-      <c r="N4">
-        <v>124324511</v>
-      </c>
-      <c r="O4" t="s">
-        <v>96</v>
-      </c>
-      <c r="P4" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>114</v>
-      </c>
-      <c r="R4" s="4">
-        <v>45292</v>
-      </c>
-      <c r="S4" s="4">
-        <v>45306</v>
-      </c>
-      <c r="T4" s="4">
-        <v>45672</v>
-      </c>
-      <c r="U4" s="4">
-        <v>45306</v>
-      </c>
-      <c r="V4" s="4">
-        <v>45672</v>
-      </c>
-      <c r="W4">
-        <v>120</v>
-      </c>
-      <c r="X4">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24">
-      <c r="A5" t="s">
-        <v>151</v>
-      </c>
-      <c r="B5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5">
-        <v>1111</v>
-      </c>
-      <c r="D5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5">
-        <v>2374188</v>
-      </c>
-      <c r="F5" t="s">
-        <v>169</v>
-      </c>
-      <c r="G5">
-        <v>0.4</v>
-      </c>
-      <c r="H5">
-        <v>5249897308</v>
-      </c>
-      <c r="I5" s="14">
-        <v>45108</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="L5">
-        <v>124324092</v>
-      </c>
-      <c r="M5" t="s">
-        <v>124</v>
-      </c>
-      <c r="N5">
-        <v>124324512</v>
-      </c>
-      <c r="O5" t="s">
-        <v>96</v>
-      </c>
-      <c r="P5" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>115</v>
-      </c>
-      <c r="R5" s="4">
-        <v>45245</v>
-      </c>
-      <c r="S5" s="4">
-        <v>45306</v>
-      </c>
-      <c r="T5" s="4">
-        <v>45672</v>
-      </c>
-      <c r="U5" s="4">
-        <v>45306</v>
-      </c>
-      <c r="V5" s="4">
-        <v>45672</v>
-      </c>
-      <c r="W5">
-        <v>120</v>
-      </c>
-      <c r="X5">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24">
-      <c r="A6" t="s">
-        <v>151</v>
-      </c>
-      <c r="B6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6">
-        <v>1111</v>
-      </c>
-      <c r="D6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6">
-        <v>6987458</v>
-      </c>
-      <c r="F6" t="s">
-        <v>169</v>
-      </c>
-      <c r="G6">
-        <v>0.3</v>
-      </c>
-      <c r="H6">
-        <v>4579088313</v>
-      </c>
-      <c r="I6" s="14">
-        <v>45108</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="L6">
-        <v>124324092</v>
-      </c>
-      <c r="M6" t="s">
-        <v>124</v>
-      </c>
-      <c r="N6">
-        <v>124324512</v>
-      </c>
-      <c r="O6" t="s">
-        <v>96</v>
-      </c>
-      <c r="P6" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>115</v>
-      </c>
-      <c r="R6" s="4">
-        <v>45245</v>
-      </c>
-      <c r="S6" s="4">
-        <v>45306</v>
-      </c>
-      <c r="T6" s="4">
-        <v>45672</v>
-      </c>
-      <c r="U6" s="4">
-        <v>45306</v>
-      </c>
-      <c r="V6" s="4">
-        <v>45672</v>
-      </c>
-      <c r="W6">
-        <v>120</v>
-      </c>
-      <c r="X6">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24">
-      <c r="A7" t="s">
-        <v>151</v>
-      </c>
-      <c r="B7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C7">
-        <v>1111</v>
-      </c>
-      <c r="D7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7">
-        <v>3693358</v>
-      </c>
-      <c r="F7" t="s">
-        <v>170</v>
-      </c>
-      <c r="G7">
-        <v>0.3</v>
-      </c>
-      <c r="H7">
-        <v>7859725531</v>
-      </c>
-      <c r="I7" s="14">
-        <v>45108</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="L7">
-        <v>124324092</v>
-      </c>
-      <c r="M7" t="s">
-        <v>124</v>
-      </c>
-      <c r="N7">
-        <v>124324512</v>
-      </c>
-      <c r="O7" t="s">
-        <v>96</v>
-      </c>
-      <c r="P7" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>115</v>
-      </c>
-      <c r="R7" s="4">
-        <v>45245</v>
-      </c>
-      <c r="S7" s="4">
-        <v>45306</v>
-      </c>
-      <c r="T7" s="4">
-        <v>45672</v>
-      </c>
-      <c r="U7" s="4">
-        <v>45306</v>
-      </c>
-      <c r="V7" s="4">
-        <v>45672</v>
-      </c>
-      <c r="W7">
-        <v>120</v>
-      </c>
-      <c r="X7">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24">
-      <c r="A8" t="s">
-        <v>147</v>
-      </c>
-      <c r="B8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8">
-        <v>1245</v>
-      </c>
-      <c r="D8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8">
-        <v>3693358</v>
-      </c>
-      <c r="F8" t="s">
-        <v>170</v>
-      </c>
-      <c r="G8">
-        <v>0.5</v>
-      </c>
-      <c r="H8">
-        <v>5260869017</v>
-      </c>
-      <c r="I8" s="14">
-        <v>45292</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="L8">
-        <v>345675387</v>
-      </c>
-      <c r="M8" t="s">
-        <v>127</v>
-      </c>
-      <c r="N8">
-        <v>345675807</v>
-      </c>
-      <c r="O8" t="s">
-        <v>91</v>
-      </c>
-      <c r="P8" t="s">
-        <v>145</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>115</v>
-      </c>
-      <c r="R8" s="4">
-        <v>45342</v>
-      </c>
-      <c r="S8" s="4">
-        <v>45306</v>
-      </c>
-      <c r="T8" s="4">
-        <v>45337</v>
-      </c>
-      <c r="U8" s="4">
-        <v>45306</v>
-      </c>
-      <c r="V8" s="4">
-        <v>45337</v>
-      </c>
-      <c r="W8">
-        <v>6</v>
-      </c>
-      <c r="X8">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24">
-      <c r="A9" t="s">
-        <v>147</v>
-      </c>
-      <c r="B9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C9">
-        <v>1245</v>
-      </c>
-      <c r="D9" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9">
-        <v>2374188</v>
-      </c>
-      <c r="F9" t="s">
-        <v>169</v>
-      </c>
-      <c r="G9">
-        <v>0.5</v>
-      </c>
-      <c r="H9">
-        <v>1292794322</v>
-      </c>
-      <c r="I9" s="14">
-        <v>45292</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="L9">
-        <v>345675387</v>
-      </c>
-      <c r="M9" t="s">
-        <v>127</v>
-      </c>
-      <c r="N9">
-        <v>345675807</v>
-      </c>
-      <c r="O9" t="s">
-        <v>91</v>
-      </c>
-      <c r="P9" t="s">
-        <v>145</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>115</v>
-      </c>
-      <c r="R9" s="4">
-        <v>45342</v>
-      </c>
-      <c r="S9" s="4">
-        <v>45306</v>
-      </c>
-      <c r="T9" s="4">
-        <v>45337</v>
-      </c>
-      <c r="U9" s="4">
-        <v>45306</v>
-      </c>
-      <c r="V9" s="4">
-        <v>45337</v>
-      </c>
-      <c r="W9">
-        <v>6</v>
-      </c>
-      <c r="X9">
-        <v>0.1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7ab8c0d4-f18b-4fef-b649-c77d178c2495">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="65efab6e-20b9-465e-9733-f0c2ab732419" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003456B0730C78B347BD7589BC061D6E7A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="eb47ff602caa7ec4c93498109dbc0598">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7ab8c0d4-f18b-4fef-b649-c77d178c2495" xmlns:ns3="65efab6e-20b9-465e-9733-f0c2ab732419" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="15d39866744b831c8a58edb1b96951e3" ns2:_="" ns3:_="">
     <xsd:import namespace="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
@@ -55022,7 +55156,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -55031,18 +55165,18 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE50E33B-922F-4D33-8831-2DF5BA7F11F6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
-    <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7ab8c0d4-f18b-4fef-b649-c77d178c2495">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="65efab6e-20b9-465e-9733-f0c2ab732419" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D43FA500-B4BA-4DED-8DE0-EA4A442F0F3F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -55061,10 +55195,21 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C685BDB-1785-4A39-A308-4CA166889A49}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE50E33B-922F-4D33-8831-2DF5BA7F11F6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
+    <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
fix: se ajustan insumos de produccion directa para componente de financiacion de decenal
</commit_message>
<xml_diff>
--- a/prototipo_pcr/inputs/insumos.xlsx
+++ b/prototipo_pcr/inputs/insumos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\proyectos_sura\Decenal\Prototipo\prototipo-pcr\prototipo_pcr\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2243AF27-2D62-4BE1-9706-CB09D188EEFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC1B003F-938C-4513-98E1-C62D6B7070E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="959" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">tasa_cambio!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">tipo_seguro!$A$1:$C$1</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcMode="manual" iterateCount="3000"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1038,7 +1038,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8963" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8964" uniqueCount="457">
   <si>
     <t>tipo_insumo</t>
   </si>
@@ -2375,19 +2375,10 @@
     <t>BAN108762414</t>
   </si>
   <si>
-    <t>produccion_directo_componente_finan</t>
-  </si>
-  <si>
     <t>003000000545</t>
   </si>
   <si>
-    <t>0030000005451</t>
-  </si>
-  <si>
     <t>RECONSTRUCCION</t>
-  </si>
-  <si>
-    <t>00300000054501</t>
   </si>
   <si>
     <t>VIVIENDA_SEGURA</t>
@@ -2409,6 +2400,15 @@
   </si>
   <si>
     <t>CO</t>
+  </si>
+  <si>
+    <t>aplica_ipc_mensual</t>
+  </si>
+  <si>
+    <t>003000000723</t>
+  </si>
+  <si>
+    <t>00300000072301</t>
   </si>
 </sst>
 </file>
@@ -16897,29 +16897,31 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BBAE1AE-0ED6-4B2E-B092-2639765DD066}">
-  <sheetPr>
-    <tabColor theme="9"/>
+  <sheetPr codeName="Hoja17">
+    <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G2" sqref="G2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.77734375" customWidth="1"/>
-    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="5" customFormat="1">
+    <row r="1" spans="1:11" s="5" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
@@ -16939,19 +16941,22 @@
         <v>75</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="I1" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>451</v>
       </c>
-      <c r="J1" s="5" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="10" customFormat="1">
+    </row>
+    <row r="2" spans="1:11" s="10" customFormat="1">
       <c r="A2" s="10" t="s">
         <v>30</v>
       </c>
@@ -16973,17 +16978,20 @@
       <c r="G2" s="10">
         <v>1</v>
       </c>
-      <c r="H2" s="10" t="s">
-        <v>456</v>
+      <c r="H2" s="10">
+        <v>1</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>452</v>
-      </c>
-      <c r="J2" s="10">
+        <v>453</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>449</v>
+      </c>
+      <c r="K2" s="10">
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="10" customFormat="1">
+    <row r="3" spans="1:11" s="10" customFormat="1">
       <c r="A3" s="10" t="s">
         <v>32</v>
       </c>
@@ -17005,13 +17013,16 @@
       <c r="G3" s="10">
         <v>1</v>
       </c>
-      <c r="H3" s="10" t="s">
-        <v>456</v>
+      <c r="H3" s="10">
+        <v>1</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>452</v>
-      </c>
-      <c r="J3" s="10">
+        <v>453</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>449</v>
+      </c>
+      <c r="K3" s="10">
         <v>120</v>
       </c>
     </row>
@@ -49513,8 +49524,8 @@
   <sheetPr codeName="Hoja6"/>
   <dimension ref="A1:V25"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U30" sqref="U30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -51141,35 +51152,35 @@
     </row>
     <row r="24" spans="1:22">
       <c r="B24" t="s">
-        <v>445</v>
+        <v>10</v>
       </c>
       <c r="C24" t="s">
         <v>13</v>
       </c>
       <c r="D24" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E24" s="4">
         <v>44733</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>447</v>
-      </c>
-      <c r="G24" s="7">
-        <v>30000005451</v>
+        <v>455</v>
+      </c>
+      <c r="G24">
+        <v>3000000723</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="I24" s="1" t="str">
         <f t="shared" si="1"/>
         <v>RECONSTRUCCION</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>449</v>
+        <v>456</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="L24" s="6" t="s">
         <v>342</v>
@@ -51178,7 +51189,7 @@
         <v>91</v>
       </c>
       <c r="N24" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="O24" t="s">
         <v>143</v>
@@ -51187,25 +51198,22 @@
         <v>115</v>
       </c>
       <c r="Q24" s="4">
-        <f>+E24</f>
-        <v>44733</v>
+        <v>45641</v>
       </c>
       <c r="R24" s="4">
-        <f>+Q24</f>
-        <v>44733</v>
+        <v>45641</v>
       </c>
       <c r="S24" s="64">
-        <v>48386</v>
+        <v>49293</v>
       </c>
       <c r="T24" s="4">
-        <f>+S24</f>
-        <v>48386</v>
+        <v>45641</v>
       </c>
       <c r="U24" s="64">
-        <v>48386</v>
+        <v>49293</v>
       </c>
       <c r="V24" s="59">
-        <v>973931014</v>
+        <v>315456190</v>
       </c>
     </row>
     <row r="25" spans="1:22">
@@ -51229,6 +51237,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91DF4D8-2AEA-4913-93D7-B86EA85C5B3E}">
+  <sheetPr codeName="Hoja18"/>
   <dimension ref="A1:W41"/>
   <sheetViews>
     <sheetView zoomScale="57" workbookViewId="0">
@@ -54956,6 +54965,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7ab8c0d4-f18b-4fef-b649-c77d178c2495">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="65efab6e-20b9-465e-9733-f0c2ab732419" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003456B0730C78B347BD7589BC061D6E7A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="eb47ff602caa7ec4c93498109dbc0598">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7ab8c0d4-f18b-4fef-b649-c77d178c2495" xmlns:ns3="65efab6e-20b9-465e-9733-f0c2ab732419" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="15d39866744b831c8a58edb1b96951e3" ns2:_="" ns3:_="">
     <xsd:import namespace="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
@@ -55156,7 +55176,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -55165,18 +55185,18 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7ab8c0d4-f18b-4fef-b649-c77d178c2495">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="65efab6e-20b9-465e-9733-f0c2ab732419" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE50E33B-922F-4D33-8831-2DF5BA7F11F6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
+    <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D43FA500-B4BA-4DED-8DE0-EA4A442F0F3F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -55195,21 +55215,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C685BDB-1785-4A39-A308-4CA166889A49}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE50E33B-922F-4D33-8831-2DF5BA7F11F6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
-    <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
fix: se incluye la moneda del documento en el cruce con parametros componente financiacion
</commit_message>
<xml_diff>
--- a/prototipo_pcr/inputs/insumos.xlsx
+++ b/prototipo_pcr/inputs/insumos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\proyectos_sura\Decenal\Prototipo\prototipo-pcr\prototipo_pcr\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC1B003F-938C-4513-98E1-C62D6B7070E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057A5D23-BD03-468E-9D5A-E61D0C745F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="959" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -548,375 +548,6 @@
 <file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Priscilla Andrea Palacios Ruiz</author>
-  </authors>
-  <commentList>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{4528A10A-A994-8442-A047-E7A1AE24EFF8}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Está completa total contrato, se abre por reasegurador con la columna porcentaje participacion reasegurador. Si ya viene abierta no es necesaria esta operación</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Priscilla Andrea Palacios Ruiz</author>
-  </authors>
-  <commentList>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{F45A81B6-76FA-6A45-BF63-3EFA4DDE4845}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Priscilla Andrea Palacios Ruiz:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>saldo constitucion / saldo liberacion / movimiento constitucion / movimiento liberacion / fluctuacion / deterioro</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments12.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={B4F53F10-94F2-0D4A-8418-EA623B88C944}</author>
-  </authors>
-  <commentList>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{B4F53F10-94F2-0D4A-8418-EA623B88C944}">
-      <text>
-        <t>[Comentario encadenado]
-Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
-Comentario:
-    Ramo decenal</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments13.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Priscilla Andrea Palacios Ruiz</author>
-  </authors>
-  <commentList>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{CC495957-854E-E645-8C7D-D273871D5F1C}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>fecha de ultima renovacion de la poliza conocida a la fecha del recibo</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Priscilla Andrea Palacios Ruiz</author>
-  </authors>
-  <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{8895739B-A3D9-984E-8E20-3A485153E90F}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Nombres Prototipo</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Priscilla Andrea Palacios Ruiz</author>
-  </authors>
-  <commentList>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{7A5C1A69-0425-664A-AD23-235D0D46F4CB}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>fecha de ultima renovacion de la poliza conocida a la fecha del recibo</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Priscilla Andrea Palacios Ruiz</author>
-  </authors>
-  <commentList>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{6646B43B-F165-4295-952A-69884C5981B2}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>fecha de ultima renovacion de la poliza conocida a la fecha del recibo</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Priscilla Andrea Palacios Ruiz</author>
-  </authors>
-  <commentList>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{0E36EDD6-5A57-9343-8130-CE65611FE131}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>fecha de ultima renovacion de la poliza conocida a la fecha del recibo</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{D9B7D91C-F7E6-7049-88D7-306E8176ED0D}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>es el recibo de la cesion al reaseguro</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{1A1486ED-68D5-E44F-B774-F7614417A941}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>la fecha negociada desde donde inicia a cubrir el contrato de reaseguro</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{41D4138C-3A2B-764D-A151-DBB640FDE563}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>debe ser la misma entre directo y rea</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AC1" authorId="0" shapeId="0" xr:uid="{615C3EE8-58D0-244B-A8A9-61E48533A4E2}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>está completa total contrato, se abre por reasegurador con la columna porcentaje participacion reasegurador. Si ya viene abierta no es necesaria esta operación</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Priscilla Andrea Palacios Ruiz</author>
-  </authors>
-  <commentList>
-    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{16C83569-8856-3941-A083-484460776B6E}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>debe ser la misma entre directo y comisiones reaseguro, pero si no lo es, traer la de la comision</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{E92E6D44-20CF-CB40-B52F-ADAAD919B98A}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>este es el más importante, no importa si se despeja de los otros valores o si viaja directamente</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Priscilla Andrea Palacios Ruiz</author>
-  </authors>
-  <commentList>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{1770F033-91D7-0047-BD15-7694292C6393}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>si es multiramo, ya debe llegar abierto por ramo</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{C8C07976-3C72-1D44-9A79-A6697E245BBC}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>puede que no tenga sentido para el no proporcional, se usan igual a las de recibo para que funcione el código. Si no existen, ajustar el código</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Priscilla Andrea Palacios Ruiz</author>
-  </authors>
-  <commentList>
-    <comment ref="C31" authorId="0" shapeId="0" xr:uid="{E2815E8B-080C-EB4D-8E74-708575AE05E6}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>A partir de este momento los limites se ajustan a las condiciones reinstaladas del contrato</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
     <author>Sebatian Tobon Echavarría</author>
     <author>Priscilla Andrea Palacios Ruiz</author>
   </authors>
@@ -1037,8 +668,411 @@
 </comments>
 </file>
 
+<file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Priscilla Andrea Palacios Ruiz</author>
+  </authors>
+  <commentList>
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{4528A10A-A994-8442-A047-E7A1AE24EFF8}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Está completa total contrato, se abre por reasegurador con la columna porcentaje participacion reasegurador. Si ya viene abierta no es necesaria esta operación</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments12.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Priscilla Andrea Palacios Ruiz</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{F45A81B6-76FA-6A45-BF63-3EFA4DDE4845}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Priscilla Andrea Palacios Ruiz:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>saldo constitucion / saldo liberacion / movimiento constitucion / movimiento liberacion / fluctuacion / deterioro</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments13.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={B4F53F10-94F2-0D4A-8418-EA623B88C944}</author>
+  </authors>
+  <commentList>
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{B4F53F10-94F2-0D4A-8418-EA623B88C944}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    Ramo decenal</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments14.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Priscilla Andrea Palacios Ruiz</author>
+  </authors>
+  <commentList>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{CC495957-854E-E645-8C7D-D273871D5F1C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>fecha de ultima renovacion de la poliza conocida a la fecha del recibo</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Priscilla</author>
+  </authors>
+  <commentList>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{FD9F9E7A-DAA6-42E8-B98F-A2E2D99C2376}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Priscilla:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No puede ser "*" (todas) pues implica curvas distintas</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Priscilla Andrea Palacios Ruiz</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{8895739B-A3D9-984E-8E20-3A485153E90F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nombres Prototipo</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Priscilla Andrea Palacios Ruiz</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{7A5C1A69-0425-664A-AD23-235D0D46F4CB}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>fecha de ultima renovacion de la poliza conocida a la fecha del recibo</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Priscilla Andrea Palacios Ruiz</author>
+  </authors>
+  <commentList>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{6646B43B-F165-4295-952A-69884C5981B2}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>fecha de ultima renovacion de la poliza conocida a la fecha del recibo</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Priscilla Andrea Palacios Ruiz</author>
+  </authors>
+  <commentList>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{0E36EDD6-5A57-9343-8130-CE65611FE131}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>fecha de ultima renovacion de la poliza conocida a la fecha del recibo</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{D9B7D91C-F7E6-7049-88D7-306E8176ED0D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>es el recibo de la cesion al reaseguro</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{1A1486ED-68D5-E44F-B774-F7614417A941}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>la fecha negociada desde donde inicia a cubrir el contrato de reaseguro</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{41D4138C-3A2B-764D-A151-DBB640FDE563}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>debe ser la misma entre directo y rea</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AC1" authorId="0" shapeId="0" xr:uid="{615C3EE8-58D0-244B-A8A9-61E48533A4E2}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>está completa total contrato, se abre por reasegurador con la columna porcentaje participacion reasegurador. Si ya viene abierta no es necesaria esta operación</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Priscilla Andrea Palacios Ruiz</author>
+  </authors>
+  <commentList>
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{16C83569-8856-3941-A083-484460776B6E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>debe ser la misma entre directo y comisiones reaseguro, pero si no lo es, traer la de la comision</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{E92E6D44-20CF-CB40-B52F-ADAAD919B98A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>este es el más importante, no importa si se despeja de los otros valores o si viaja directamente</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Priscilla Andrea Palacios Ruiz</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{1770F033-91D7-0047-BD15-7694292C6393}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>si es multiramo, ya debe llegar abierto por ramo</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{C8C07976-3C72-1D44-9A79-A6697E245BBC}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>puede que no tenga sentido para el no proporcional, se usan igual a las de recibo para que funcione el código. Si no existen, ajustar el código</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Priscilla Andrea Palacios Ruiz</author>
+  </authors>
+  <commentList>
+    <comment ref="C31" authorId="0" shapeId="0" xr:uid="{E2815E8B-080C-EB4D-8E74-708575AE05E6}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>A partir de este momento los limites se ajustan a las condiciones reinstaladas del contrato</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8964" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8967" uniqueCount="457">
   <si>
     <t>tipo_insumo</t>
   </si>
@@ -2423,7 +2457,7 @@
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2562,6 +2596,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -16896,14 +16943,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BBAE1AE-0ED6-4B2E-B092-2639765DD066}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BBAE1AE-0ED6-4B2E-B092-2639765DD066}">
   <sheetPr codeName="Hoja17">
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -16914,14 +16961,15 @@
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5546875" customWidth="1"/>
+    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1">
+    <row r="1" spans="1:12" s="5" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
@@ -16941,22 +16989,25 @@
         <v>75</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>450</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>454</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>452</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>448</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="10" customFormat="1">
+    <row r="2" spans="1:12" s="10" customFormat="1">
       <c r="A2" s="10" t="s">
         <v>30</v>
       </c>
@@ -16975,23 +17026,26 @@
       <c r="F2" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="G2" s="10">
-        <v>1</v>
+      <c r="G2" s="10" t="s">
+        <v>115</v>
       </c>
       <c r="H2" s="10">
         <v>1</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="10">
+        <v>1</v>
+      </c>
+      <c r="J2" s="10" t="s">
         <v>453</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="K2" s="10" t="s">
         <v>449</v>
       </c>
-      <c r="K2" s="10">
+      <c r="L2" s="10">
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="10" customFormat="1">
+    <row r="3" spans="1:12" s="10" customFormat="1">
       <c r="A3" s="10" t="s">
         <v>32</v>
       </c>
@@ -17010,25 +17064,29 @@
       <c r="F3" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="G3" s="10">
-        <v>1</v>
+      <c r="G3" s="10" t="s">
+        <v>115</v>
       </c>
       <c r="H3" s="10">
         <v>1</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="10">
+        <v>1</v>
+      </c>
+      <c r="J3" s="10" t="s">
         <v>453</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="K3" s="10" t="s">
         <v>449</v>
       </c>
-      <c r="K3" s="10">
+      <c r="L3" s="10">
         <v>120</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -54965,17 +55023,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7ab8c0d4-f18b-4fef-b649-c77d178c2495">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="65efab6e-20b9-465e-9733-f0c2ab732419" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003456B0730C78B347BD7589BC061D6E7A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="eb47ff602caa7ec4c93498109dbc0598">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7ab8c0d4-f18b-4fef-b649-c77d178c2495" xmlns:ns3="65efab6e-20b9-465e-9733-f0c2ab732419" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="15d39866744b831c8a58edb1b96951e3" ns2:_="" ns3:_="">
     <xsd:import namespace="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
@@ -55176,6 +55223,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7ab8c0d4-f18b-4fef-b649-c77d178c2495">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="65efab6e-20b9-465e-9733-f0c2ab732419" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -55186,17 +55244,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE50E33B-922F-4D33-8831-2DF5BA7F11F6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
-    <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D43FA500-B4BA-4DED-8DE0-EA4A442F0F3F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -55215,6 +55262,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE50E33B-922F-4D33-8831-2DF5BA7F11F6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
+    <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C685BDB-1785-4A39-A308-4CA166889A49}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
fix: ajustada fecha de emision de la poliza de decenal
</commit_message>
<xml_diff>
--- a/prototipo_pcr/inputs/insumos.xlsx
+++ b/prototipo_pcr/inputs/insumos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\proyectos_sura\Decenal\Prototipo\prototipo-pcr\prototipo_pcr\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057A5D23-BD03-468E-9D5A-E61D0C745F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4ED883C-6C38-41AA-934C-25F2C6F515BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="959" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">comision_rea!$A$1:$V$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">componente_inversion_directo!$A$1:$W$37</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">gastos!$B$1:$K$221</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">gastos!$A$1:$M$245</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">map_bt!$A$1:$I$261</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">param_contabilidad!$A$1:$J$86</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">porc_descuento!$A$1:$N$17</definedName>
@@ -44,7 +44,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">tasa_cambio!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">tipo_seguro!$A$1:$C$1</definedName>
   </definedNames>
-  <calcPr calcId="191028" calcMode="manual" iterateCount="3000"/>
+  <calcPr calcId="191028" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -789,7 +789,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Priscilla:</t>
         </r>
@@ -798,10 +798,10 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-No puede ser "*" (todas) pues implica curvas distintas</t>
+No puede ser "*" (todas) pues implica usar curvas distintas</t>
         </r>
       </text>
     </comment>
@@ -1072,7 +1072,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8967" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8968" uniqueCount="458">
   <si>
     <t>tipo_insumo</t>
   </si>
@@ -2444,6 +2444,9 @@
   <si>
     <t>00300000072301</t>
   </si>
+  <si>
+    <t>decenal_financiacion</t>
+  </si>
 </sst>
 </file>
 
@@ -2601,14 +2604,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -3105,7 +3108,7 @@
   <dimension ref="A1:K89"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23:G25"/>
+      <selection activeCell="B78" sqref="B78:B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -16950,13 +16953,13 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.77734375" bestFit="1" customWidth="1"/>
@@ -17099,7 +17102,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.21875" defaultRowHeight="14.4"/>
@@ -49582,8 +49585,8 @@
   <sheetPr codeName="Hoja6"/>
   <dimension ref="A1:V25"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U30" sqref="U30"/>
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -51209,6 +51212,9 @@
       </c>
     </row>
     <row r="24" spans="1:22">
+      <c r="A24" t="s">
+        <v>457</v>
+      </c>
       <c r="B24" t="s">
         <v>10</v>
       </c>
@@ -51219,7 +51225,7 @@
         <v>445</v>
       </c>
       <c r="E24" s="4">
-        <v>44733</v>
+        <v>45641</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>455</v>
@@ -55023,6 +55029,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7ab8c0d4-f18b-4fef-b649-c77d178c2495">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="65efab6e-20b9-465e-9733-f0c2ab732419" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003456B0730C78B347BD7589BC061D6E7A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="eb47ff602caa7ec4c93498109dbc0598">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7ab8c0d4-f18b-4fef-b649-c77d178c2495" xmlns:ns3="65efab6e-20b9-465e-9733-f0c2ab732419" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="15d39866744b831c8a58edb1b96951e3" ns2:_="" ns3:_="">
     <xsd:import namespace="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
@@ -55223,27 +55249,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7ab8c0d4-f18b-4fef-b649-c77d178c2495">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="65efab6e-20b9-465e-9733-f0c2ab732419" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE50E33B-922F-4D33-8831-2DF5BA7F11F6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
+    <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C685BDB-1785-4A39-A308-4CA166889A49}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D43FA500-B4BA-4DED-8DE0-EA4A442F0F3F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -55262,25 +55287,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE50E33B-922F-4D33-8831-2DF5BA7F11F6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7ab8c0d4-f18b-4fef-b649-c77d178c2495"/>
-    <ds:schemaRef ds:uri="65efab6e-20b9-465e-9733-f0c2ab732419"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C685BDB-1785-4A39-A308-4CA166889A49}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{3c0bd4fe-1111-4d13-8e0c-7c33b9eb7581}" enabled="0" method="" siteId="{3c0bd4fe-1111-4d13-8e0c-7c33b9eb7581}" removed="1"/>

</xml_diff>